<commit_message>
creating html folder to combine all htmls into one; uploading Asels's html and js code
</commit_message>
<xml_diff>
--- a/Manpower_Calculation_Starbucks_Team.xlsx
+++ b/Manpower_Calculation_Starbucks_Team.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aconnolly\Documents\Bootcamp\Is_Starbucks_your_cup_of_coffee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278D0B97-FA18-4572-97A0-87821397EDAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A18744-C1CB-45E7-A841-518F566AE602}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCD9D9D5-993F-4FDB-B545-D115C471AC5E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Time in minutes</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Projected Time (hrs)</t>
+  </si>
+  <si>
+    <t>4. Readme file</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,8 +255,23 @@
       <name val="Algerian"/>
       <family val="5"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +307,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -629,7 +653,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -697,8 +721,6 @@
     <xf numFmtId="164" fontId="8" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -712,6 +734,11 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -1032,10 +1059,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1051,20 +1078,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -1123,7 +1150,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="33"/>
       <c r="E4" s="33"/>
       <c r="F4" s="33"/>
@@ -1141,7 +1168,7 @@
       <c r="B5" s="34">
         <v>36</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="47">
         <v>36</v>
       </c>
       <c r="D5" s="34">
@@ -1154,7 +1181,7 @@
       <c r="G5" s="34">
         <v>36</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="44">
         <f>SUM(B5:G5)</f>
         <v>180</v>
       </c>
@@ -1179,14 +1206,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="34"/>
-      <c r="C6" s="34">
+      <c r="C6" s="47">
         <v>20</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
-      <c r="H6" s="35">
+      <c r="H6" s="44">
         <f>SUM(B6:G6)</f>
         <v>20</v>
       </c>
@@ -1211,14 +1238,14 @@
         <v>36</v>
       </c>
       <c r="B7" s="34"/>
-      <c r="C7" s="34">
+      <c r="C7" s="47">
         <v>20</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
-      <c r="H7" s="35">
+      <c r="H7" s="44">
         <f t="shared" ref="H7" si="2">SUM(B7:G7)</f>
         <v>20</v>
       </c>
@@ -1239,26 +1266,35 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
+      <c r="A8" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
+      <c r="C8" s="47">
+        <v>40</v>
+      </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
-      <c r="H8" s="35">
+      <c r="H8" s="44">
         <f t="shared" ref="H8:H35" si="4">SUM(B8:G8)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I8" s="27">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="27"/>
-      <c r="K8" s="28"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J8" s="27">
+        <v>60</v>
+      </c>
+      <c r="K8" s="28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="L8" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1266,7 +1302,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
@@ -1282,14 +1318,14 @@
         <v>38</v>
       </c>
       <c r="B10" s="34"/>
-      <c r="C10" s="34">
+      <c r="C10" s="47">
         <v>15</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
-      <c r="H10" s="35">
+      <c r="H10" s="44">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
@@ -1316,7 +1352,7 @@
       <c r="B11" s="34">
         <v>5</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="47">
         <v>5</v>
       </c>
       <c r="D11" s="34">
@@ -1329,7 +1365,7 @@
       <c r="G11" s="34">
         <v>5</v>
       </c>
-      <c r="H11" s="35">
+      <c r="H11" s="44">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
@@ -1356,7 +1392,7 @@
       <c r="B12" s="34">
         <v>10</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="47">
         <v>10</v>
       </c>
       <c r="D12" s="34">
@@ -1369,7 +1405,7 @@
       <c r="G12" s="34">
         <v>10</v>
       </c>
-      <c r="H12" s="35">
+      <c r="H12" s="44">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
@@ -1392,12 +1428,12 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="15"/>
       <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
-      <c r="H13" s="35">
+      <c r="H13" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1417,7 +1453,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
+      <c r="C14" s="46"/>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
@@ -1433,14 +1469,14 @@
         <v>24</v>
       </c>
       <c r="B15" s="34"/>
-      <c r="C15" s="34">
+      <c r="C15" s="47">
         <v>20</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
       <c r="F15" s="34"/>
       <c r="G15" s="34"/>
-      <c r="H15" s="35">
+      <c r="H15" s="44">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
@@ -1465,14 +1501,14 @@
         <v>25</v>
       </c>
       <c r="B16" s="34"/>
-      <c r="C16" s="34">
+      <c r="C16" s="47">
         <v>5</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
-      <c r="H16" s="35">
+      <c r="H16" s="44">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
@@ -1497,14 +1533,14 @@
         <v>26</v>
       </c>
       <c r="B17" s="34"/>
-      <c r="C17" s="34">
+      <c r="C17" s="47">
         <v>120</v>
       </c>
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
-      <c r="H17" s="35">
+      <c r="H17" s="44">
         <f t="shared" si="4"/>
         <v>120</v>
       </c>
@@ -1527,12 +1563,12 @@
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="17"/>
       <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
-      <c r="H18" s="35">
+      <c r="H18" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1552,7 +1588,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
@@ -1568,14 +1604,14 @@
         <v>27</v>
       </c>
       <c r="B20" s="34"/>
-      <c r="C20" s="34">
+      <c r="C20" s="47">
         <v>250</v>
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
-      <c r="H20" s="35">
+      <c r="H20" s="44">
         <f t="shared" si="4"/>
         <v>250</v>
       </c>
@@ -1601,12 +1637,12 @@
         <v>28</v>
       </c>
       <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
-      <c r="H21" s="35">
+      <c r="H21" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1631,14 +1667,14 @@
         <v>29</v>
       </c>
       <c r="B22" s="34"/>
-      <c r="C22" s="34">
+      <c r="C22" s="47">
         <v>45</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
-      <c r="H22" s="35">
+      <c r="H22" s="44">
         <f t="shared" si="4"/>
         <v>45</v>
       </c>
@@ -1661,12 +1697,12 @@
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="34"/>
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
-      <c r="H23" s="35">
+      <c r="H23" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1689,7 +1725,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="33"/>
@@ -1705,12 +1741,12 @@
         <v>30</v>
       </c>
       <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
+      <c r="C25" s="47"/>
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
       <c r="F25" s="34"/>
       <c r="G25" s="34"/>
-      <c r="H25" s="35">
+      <c r="H25" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1733,14 +1769,14 @@
         <v>31</v>
       </c>
       <c r="B26" s="34"/>
-      <c r="C26" s="34">
+      <c r="C26" s="47">
         <v>30</v>
       </c>
       <c r="D26" s="34"/>
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
       <c r="G26" s="34"/>
-      <c r="H26" s="35">
+      <c r="H26" s="44">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
@@ -1763,12 +1799,12 @@
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="17"/>
       <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
+      <c r="C27" s="47"/>
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
-      <c r="H27" s="35">
+      <c r="H27" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1791,7 +1827,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
       <c r="F28" s="33"/>
@@ -1812,7 +1848,7 @@
       <c r="E29" s="34"/>
       <c r="F29" s="34"/>
       <c r="G29" s="34"/>
-      <c r="H29" s="35">
+      <c r="H29" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1842,7 +1878,7 @@
       <c r="E30" s="34"/>
       <c r="F30" s="34"/>
       <c r="G30" s="34"/>
-      <c r="H30" s="35">
+      <c r="H30" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1870,7 +1906,7 @@
       <c r="E31" s="34"/>
       <c r="F31" s="34"/>
       <c r="G31" s="34"/>
-      <c r="H31" s="35">
+      <c r="H31" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1914,7 +1950,7 @@
       <c r="E33" s="34"/>
       <c r="F33" s="34"/>
       <c r="G33" s="34"/>
-      <c r="H33" s="35">
+      <c r="H33" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1944,7 +1980,7 @@
       <c r="E34" s="34"/>
       <c r="F34" s="34"/>
       <c r="G34" s="34"/>
-      <c r="H34" s="35">
+      <c r="H34" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1972,11 +2008,11 @@
       <c r="E35" s="34"/>
       <c r="F35" s="34"/>
       <c r="G35" s="34"/>
-      <c r="H35" s="36">
+      <c r="H35" s="45">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I35" s="37">
+      <c r="I35" s="35">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1994,53 +2030,53 @@
       <c r="A36" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="38">
-        <f>SUM(B5:B34)</f>
+      <c r="B36" s="36">
+        <f t="shared" ref="B36:G36" si="5">SUM(B5:B34)</f>
         <v>51</v>
       </c>
-      <c r="C36" s="38">
-        <f>SUM(C5:C34)</f>
-        <v>576</v>
-      </c>
-      <c r="D36" s="38">
-        <f>SUM(D5:D34)</f>
+      <c r="C36" s="36">
+        <f t="shared" si="5"/>
+        <v>616</v>
+      </c>
+      <c r="D36" s="36">
+        <f t="shared" si="5"/>
         <v>51</v>
       </c>
-      <c r="E36" s="38">
-        <f>SUM(E5:E34)</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="38">
-        <f>SUM(F5:F34)</f>
+      <c r="E36" s="36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="36">
+        <f t="shared" si="5"/>
         <v>51</v>
       </c>
-      <c r="G36" s="39">
-        <f>SUM(G5:G34)</f>
+      <c r="G36" s="37">
+        <f t="shared" si="5"/>
         <v>51</v>
       </c>
-      <c r="H36" s="40">
+      <c r="H36" s="38">
         <f>SUM(H5:H35)</f>
-        <v>780</v>
-      </c>
-      <c r="I36" s="41">
+        <v>820</v>
+      </c>
+      <c r="I36" s="39">
         <f>SUM(I5:I35)</f>
-        <v>13</v>
-      </c>
-      <c r="J36" s="42">
+        <v>13.666666666666668</v>
+      </c>
+      <c r="J36" s="40">
         <f>SUM(J4:J35)</f>
-        <v>1310</v>
-      </c>
-      <c r="K36" s="43">
+        <v>1370</v>
+      </c>
+      <c r="K36" s="41">
         <f>SUM(K4:K35)</f>
-        <v>21.833333333333332</v>
-      </c>
-      <c r="L36" s="43">
+        <v>22.833333333333332</v>
+      </c>
+      <c r="L36" s="41">
         <f>SUM(L4:L35)</f>
-        <v>8.8333333333333321</v>
+        <v>9.1666666666666661</v>
       </c>
       <c r="M36" s="1">
         <f>SUM(B36:G36)</f>
-        <v>780</v>
+        <v>820</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.35">
@@ -2060,6 +2096,16 @@
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
         <v>3</v>
+      </c>
+      <c r="M39" s="48">
+        <f>4*4</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M40" s="1">
+        <f>M39*60</f>
+        <v>960</v>
       </c>
     </row>
   </sheetData>

</xml_diff>